<commit_message>
Update of dataset with gpt4omini
</commit_message>
<xml_diff>
--- a/doc/template/template.xlsx
+++ b/doc/template/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="139">
   <si>
     <t xml:space="preserve">ISO37101 assessment</t>
   </si>
@@ -67,9 +67,15 @@
     <t xml:space="preserve">Well Being</t>
   </si>
   <si>
+    <t xml:space="preserve">Reviewed</t>
+  </si>
+  <si>
     <t xml:space="preserve">Review</t>
   </si>
   <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
     <t xml:space="preserve">LL</t>
   </si>
   <si>
@@ -179,9 +185,6 @@
   </si>
   <si>
     <t xml:space="preserve">Activity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Title</t>
   </si>
   <si>
     <t xml:space="preserve">ID:</t>
@@ -1527,7 +1530,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1536,6 +1539,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1605,6 +1612,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2261,13 +2272,13 @@
     <tabColor rgb="FF000000"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="B2:V37"/>
+  <dimension ref="B2:W37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T9" activeCellId="0" sqref="T9:Z14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.71"/>
@@ -2277,712 +2288,719 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="7" style="0" width="8.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="2.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="85.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="12.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="15.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="8.89"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="5" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="6"/>
-      <c r="C5" s="4"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="F6" s="9" t="s">
+      <c r="C6" s="9"/>
+      <c r="F6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="F8" s="15" t="s">
+      <c r="C8" s="15"/>
+      <c r="F8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="17" t="s">
+      <c r="H8" s="17"/>
+      <c r="I8" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="17"/>
-      <c r="K8" s="18" t="s">
+      <c r="J8" s="18"/>
+      <c r="K8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18" t="s">
+      <c r="L8" s="19"/>
+      <c r="M8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="N8" s="18"/>
-      <c r="O8" s="16" t="s">
+      <c r="N8" s="19"/>
+      <c r="O8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16" t="s">
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="R8" s="16"/>
-      <c r="U8" s="19" t="s">
+      <c r="R8" s="17"/>
+      <c r="T8" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="V8" s="19" t="s">
+      <c r="U8" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="V8" s="21" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="20" t="s">
+      <c r="W8" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="20" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="N9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="O9" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="P9" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q9" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="R9" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="13" t="s">
+      <c r="C9" s="15"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="F10" s="23" t="str">
+      <c r="H9" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q9" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="R9" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="F10" s="25" t="str">
         <f aca="false">LEFT(Definitions!B12,25)&amp;"…"</f>
         <v>Governance, empowerment a…</v>
       </c>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="26"/>
-      <c r="C11" s="12"/>
-      <c r="F11" s="23" t="str">
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="28"/>
+      <c r="C11" s="13"/>
+      <c r="F11" s="25" t="str">
         <f aca="false">LEFT(Definitions!B13,25)&amp;"…"</f>
         <v>Education and capacity bu…</v>
       </c>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="F12" s="23" t="str">
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="F12" s="25" t="str">
         <f aca="false">LEFT(Definitions!B14,25)&amp;"…"</f>
         <v>Innovation, creativity an…</v>
       </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="27"/>
-      <c r="C13" s="14"/>
-      <c r="F13" s="23" t="str">
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="27"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="29"/>
+      <c r="C13" s="15"/>
+      <c r="F13" s="25" t="str">
         <f aca="false">LEFT(Definitions!B15,25)&amp;"…"</f>
         <v>Health and care in the co…</v>
       </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="27"/>
-      <c r="C14" s="14"/>
-      <c r="F14" s="23" t="str">
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="27"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="29"/>
+      <c r="C14" s="15"/>
+      <c r="F14" s="25" t="str">
         <f aca="false">LEFT(Definitions!B16,25)&amp;"…"</f>
         <v>Culture and community ide…</v>
       </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="26"/>
-      <c r="C15" s="12"/>
-      <c r="F15" s="23" t="str">
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="27"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="28"/>
+      <c r="C15" s="13"/>
+      <c r="F15" s="25" t="str">
         <f aca="false">LEFT(Definitions!B17,25)&amp;"…"</f>
         <v>Living together, interdep…</v>
       </c>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="F16" s="23" t="str">
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="27"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="F16" s="25" t="str">
         <f aca="false">LEFT(Definitions!B18,25)&amp;"…"</f>
         <v>Economy and sustainable p…</v>
       </c>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="27"/>
-      <c r="C17" s="14"/>
-      <c r="F17" s="23" t="str">
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="27"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="29"/>
+      <c r="C17" s="15"/>
+      <c r="F17" s="25" t="str">
         <f aca="false">LEFT(Definitions!B19,25)&amp;"…"</f>
         <v>Living and working enviro…</v>
       </c>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25" t="n">
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27" t="n">
         <v>5</v>
       </c>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="27"/>
-      <c r="C18" s="14"/>
-      <c r="F18" s="23" t="str">
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="27"/>
+      <c r="R17" s="27"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="29"/>
+      <c r="C18" s="15"/>
+      <c r="F18" s="25" t="str">
         <f aca="false">LEFT(Definitions!B20,25)&amp;"…"</f>
         <v>Safety and security…</v>
       </c>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25" t="n">
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="25"/>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="28"/>
-      <c r="C19" s="12"/>
-      <c r="F19" s="23" t="str">
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="27"/>
+      <c r="R18" s="27"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="30"/>
+      <c r="C19" s="13"/>
+      <c r="F19" s="25" t="str">
         <f aca="false">LEFT(Definitions!B21,25)&amp;"…"</f>
         <v>Biodiversity and ecosyste…</v>
       </c>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="25" t="n">
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="25"/>
-      <c r="R19" s="25"/>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="F20" s="23" t="str">
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="27"/>
+      <c r="R19" s="27"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="F20" s="25" t="str">
         <f aca="false">LEFT(Definitions!B22,25)&amp;"…"</f>
         <v>Community smart infrastru…</v>
       </c>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="25" t="n">
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27" t="n">
         <v>3</v>
       </c>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="25"/>
-      <c r="R20" s="25"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="27"/>
-      <c r="C21" s="14"/>
-      <c r="F21" s="23" t="str">
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="29"/>
+      <c r="C21" s="15"/>
+      <c r="F21" s="25" t="str">
         <f aca="false">LEFT(Definitions!B23,25)&amp;"…"</f>
         <v>Mobility…</v>
       </c>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="25"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="27"/>
-      <c r="C22" s="14"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="29"/>
+      <c r="C22" s="15"/>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="F24" s="15" t="s">
+      <c r="B24" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="G24" s="16" t="s">
+      <c r="C24" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="16"/>
-      <c r="I24" s="17" t="s">
+      <c r="H24" s="17"/>
+      <c r="I24" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="J24" s="17"/>
-      <c r="K24" s="18" t="s">
+      <c r="J24" s="18"/>
+      <c r="K24" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18" t="s">
+      <c r="L24" s="19"/>
+      <c r="M24" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="N24" s="18"/>
-      <c r="O24" s="16" t="s">
+      <c r="N24" s="19"/>
+      <c r="O24" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16" t="s">
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="R24" s="16"/>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F25" s="15"/>
-      <c r="G25" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J25" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="K25" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="L25" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="M25" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="N25" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="O25" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="P25" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q25" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="R25" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F26" s="23" t="str">
+      <c r="R24" s="17"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F25" s="16"/>
+      <c r="G25" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="K25" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="L25" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="M25" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="N25" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="O25" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="P25" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q25" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="R25" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F26" s="25" t="str">
         <f aca="false">F10</f>
         <v>Governance, empowerment a…</v>
       </c>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="25"/>
-      <c r="R26" s="25"/>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F27" s="23" t="str">
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="27"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="27"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F27" s="25" t="str">
         <f aca="false">F11</f>
         <v>Education and capacity bu…</v>
       </c>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="25" t="n">
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="27"/>
+      <c r="N27" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="25"/>
-      <c r="R27" s="25"/>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F28" s="23" t="str">
+      <c r="O27" s="26"/>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="27"/>
+      <c r="R27" s="27"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F28" s="25" t="str">
         <f aca="false">F12</f>
         <v>Innovation, creativity an…</v>
       </c>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="25" t="n">
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="O28" s="24"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="25"/>
-      <c r="R28" s="25"/>
-    </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F29" s="23" t="str">
+      <c r="O28" s="26"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="27"/>
+      <c r="R28" s="27"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F29" s="25" t="str">
         <f aca="false">F13</f>
         <v>Health and care in the co…</v>
       </c>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="25" t="n">
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="27" t="n">
         <v>3</v>
       </c>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="25"/>
-      <c r="R29" s="25"/>
-    </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F30" s="23" t="str">
+      <c r="O29" s="26"/>
+      <c r="P29" s="26"/>
+      <c r="Q29" s="27"/>
+      <c r="R29" s="27"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F30" s="25" t="str">
         <f aca="false">F14</f>
         <v>Culture and community ide…</v>
       </c>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="25" t="n">
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="27"/>
+      <c r="N30" s="27" t="n">
         <v>4</v>
       </c>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="25"/>
-      <c r="R30" s="25"/>
-    </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F31" s="23" t="str">
+      <c r="O30" s="26"/>
+      <c r="P30" s="26"/>
+      <c r="Q30" s="27"/>
+      <c r="R30" s="27"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F31" s="25" t="str">
         <f aca="false">F15</f>
         <v>Living together, interdep…</v>
       </c>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="25" t="n">
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="27"/>
+      <c r="N31" s="27" t="n">
         <v>5</v>
       </c>
-      <c r="O31" s="24"/>
-      <c r="P31" s="24"/>
-      <c r="Q31" s="25"/>
-      <c r="R31" s="25"/>
-    </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F32" s="23" t="str">
+      <c r="O31" s="26"/>
+      <c r="P31" s="26"/>
+      <c r="Q31" s="27"/>
+      <c r="R31" s="27"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F32" s="25" t="str">
         <f aca="false">F16</f>
         <v>Economy and sustainable p…</v>
       </c>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="25"/>
-      <c r="N32" s="25"/>
-      <c r="O32" s="24"/>
-      <c r="P32" s="24"/>
-      <c r="Q32" s="25"/>
-      <c r="R32" s="25"/>
-    </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F33" s="23" t="str">
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="27"/>
+      <c r="N32" s="27"/>
+      <c r="O32" s="26"/>
+      <c r="P32" s="26"/>
+      <c r="Q32" s="27"/>
+      <c r="R32" s="27"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F33" s="25" t="str">
         <f aca="false">F17</f>
         <v>Living and working enviro…</v>
       </c>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="24"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="25"/>
-      <c r="O33" s="24"/>
-      <c r="P33" s="24"/>
-      <c r="Q33" s="25"/>
-      <c r="R33" s="25"/>
-    </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F34" s="23" t="str">
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="27"/>
+      <c r="N33" s="27"/>
+      <c r="O33" s="26"/>
+      <c r="P33" s="26"/>
+      <c r="Q33" s="27"/>
+      <c r="R33" s="27"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F34" s="25" t="str">
         <f aca="false">F18</f>
         <v>Safety and security…</v>
       </c>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="24"/>
-      <c r="M34" s="25"/>
-      <c r="N34" s="25"/>
-      <c r="O34" s="24"/>
-      <c r="P34" s="24"/>
-      <c r="Q34" s="25"/>
-      <c r="R34" s="25"/>
-    </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F35" s="23" t="str">
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="26"/>
+      <c r="L34" s="26"/>
+      <c r="M34" s="27"/>
+      <c r="N34" s="27"/>
+      <c r="O34" s="26"/>
+      <c r="P34" s="26"/>
+      <c r="Q34" s="27"/>
+      <c r="R34" s="27"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F35" s="25" t="str">
         <f aca="false">F19</f>
         <v>Biodiversity and ecosyste…</v>
       </c>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="24"/>
-      <c r="L35" s="24"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="25"/>
-      <c r="O35" s="24"/>
-      <c r="P35" s="24"/>
-      <c r="Q35" s="25"/>
-      <c r="R35" s="25"/>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F36" s="23" t="str">
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="26"/>
+      <c r="L35" s="26"/>
+      <c r="M35" s="27"/>
+      <c r="N35" s="27"/>
+      <c r="O35" s="26"/>
+      <c r="P35" s="26"/>
+      <c r="Q35" s="27"/>
+      <c r="R35" s="27"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F36" s="25" t="str">
         <f aca="false">F20</f>
         <v>Community smart infrastru…</v>
       </c>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="24"/>
-      <c r="L36" s="24"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="24"/>
-      <c r="P36" s="24"/>
-      <c r="Q36" s="25"/>
-      <c r="R36" s="25"/>
-    </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F37" s="23" t="str">
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="26"/>
+      <c r="M36" s="27"/>
+      <c r="N36" s="27"/>
+      <c r="O36" s="26"/>
+      <c r="P36" s="26"/>
+      <c r="Q36" s="27"/>
+      <c r="R36" s="27"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F37" s="25" t="str">
         <f aca="false">F21</f>
         <v>Mobility…</v>
       </c>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="24"/>
-      <c r="L37" s="24"/>
-      <c r="M37" s="25"/>
-      <c r="N37" s="25"/>
-      <c r="O37" s="24"/>
-      <c r="P37" s="24"/>
-      <c r="Q37" s="25"/>
-      <c r="R37" s="25"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="26"/>
+      <c r="M37" s="27"/>
+      <c r="N37" s="27"/>
+      <c r="O37" s="26"/>
+      <c r="P37" s="26"/>
+      <c r="Q37" s="27"/>
+      <c r="R37" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -3018,7 +3036,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{1822D06F-B35F-40EE-9DA4-AA10151F96E8}">
+          <x14:cfRule type="iconSet" priority="2" id="{9BEFD5C9-5633-4D32-9386-232BECF2F62B}">
             <x14:iconSet iconSet="3Stars" reverse="0" showValue="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3034,7 +3052,7 @@
           <xm:sqref>G10:R21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="3" id="{3A7BC291-91B4-47B3-A369-9BF5FFEB62C8}">
+          <x14:cfRule type="iconSet" priority="3" id="{2E6FEA75-9989-4B98-A174-E9E24774F836}">
             <x14:iconSet iconSet="5Boxes" reverse="0" showValue="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3070,123 +3088,123 @@
   <dimension ref="B1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
+      <selection pane="topLeft" activeCell="M15" activeCellId="1" sqref="T9:Z14 M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="31" width="41.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="33" width="41.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="32" t="s">
-        <v>24</v>
+      <c r="C1" s="34" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="34" t="s">
-        <v>26</v>
+      <c r="B3" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>28</v>
+      <c r="B4" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>30</v>
+      <c r="B5" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>32</v>
+      <c r="B6" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="37"/>
-      <c r="C7" s="39" t="s">
-        <v>33</v>
+      <c r="B7" s="39"/>
+      <c r="C7" s="41" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>35</v>
+      <c r="B8" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>37</v>
+      <c r="B9" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="41" t="s">
-        <v>39</v>
+      <c r="B10" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="42" t="s">
+      <c r="B12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="44" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="43" t="s">
-        <v>42</v>
+      <c r="B13" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="44" t="s">
-        <v>44</v>
+      <c r="B14" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="44" t="s">
-        <v>46</v>
+      <c r="B15" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="46" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="45" t="s">
-        <v>48</v>
+      <c r="B16" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="47" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3211,1268 +3229,1270 @@
     <tabColor rgb="FFC5E0B4"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="B1:N51"/>
+  <dimension ref="B1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q26" activeCellId="0" sqref="Q26"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AMJ16" activeCellId="1" sqref="T9:Z14 AMJ16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="3.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="16" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="16" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1024" min="20" style="0" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
+      <c r="B4" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="K5" s="49"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
+      <c r="B5" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="51"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="49" t="s">
+      <c r="B6" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="K6" s="49"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="48"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="K6" s="51"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="52" t="s">
+      <c r="B7" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="K7" s="52"/>
-      <c r="L7" s="48"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="48"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" s="54"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
     </row>
     <row r="8" customFormat="false" ht="300.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="53"/>
+      <c r="B8" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
     </row>
     <row r="9" customFormat="false" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="54" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="54" t="s">
+      <c r="B10" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="54" t="s">
+      <c r="C10" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="46" t="s">
+      <c r="D10" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="46"/>
-      <c r="N10" s="46"/>
+      <c r="E10" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="55"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="57"/>
-      <c r="N11" s="57"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="59"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="55"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="57"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="59"/>
+      <c r="M12" s="59"/>
+      <c r="N12" s="59"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="55"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="57"/>
-      <c r="N13" s="57"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="59"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="55"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="57"/>
-      <c r="N14" s="57"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="59"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="55"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="57"/>
-      <c r="M15" s="57"/>
-      <c r="N15" s="57"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="59"/>
+      <c r="N15" s="59"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="55"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="57"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="59"/>
+      <c r="N16" s="59"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="55"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="57"/>
-      <c r="K17" s="57"/>
-      <c r="L17" s="57"/>
-      <c r="M17" s="57"/>
-      <c r="N17" s="57"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="59"/>
+      <c r="M17" s="59"/>
+      <c r="N17" s="59"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="55"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="57"/>
-      <c r="N18" s="57"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="59"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="59"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="55"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="57"/>
-      <c r="M19" s="57"/>
-      <c r="N19" s="57"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="55"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="57"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="57"/>
-      <c r="N20" s="57"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="59"/>
+      <c r="J20" s="59"/>
+      <c r="K20" s="59"/>
+      <c r="L20" s="59"/>
+      <c r="M20" s="59"/>
+      <c r="N20" s="59"/>
     </row>
     <row r="21" customFormat="false" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="59" t="s">
+      <c r="B22" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="59"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="59"/>
-      <c r="H22" s="59"/>
-      <c r="I22" s="60" t="s">
+      <c r="C22" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="J22" s="60"/>
-      <c r="K22" s="60"/>
-      <c r="L22" s="60"/>
-      <c r="M22" s="60"/>
-      <c r="N22" s="60"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="J22" s="62"/>
+      <c r="K22" s="62"/>
+      <c r="L22" s="62"/>
+      <c r="M22" s="62"/>
+      <c r="N22" s="62"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="58"/>
-      <c r="C23" s="61" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="61" t="s">
+      <c r="B23" s="60"/>
+      <c r="C23" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="J23" s="61"/>
-      <c r="K23" s="61"/>
-      <c r="L23" s="61"/>
-      <c r="M23" s="61"/>
-      <c r="N23" s="61"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="63"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="J23" s="63"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="63"/>
+      <c r="M23" s="63"/>
+      <c r="N23" s="63"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="58"/>
-      <c r="C24" s="61" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="62" t="s">
+      <c r="B24" s="60"/>
+      <c r="C24" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="J24" s="62"/>
-      <c r="K24" s="62"/>
-      <c r="L24" s="62"/>
-      <c r="M24" s="62"/>
-      <c r="N24" s="62"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="63"/>
+      <c r="G24" s="63"/>
+      <c r="H24" s="63"/>
+      <c r="I24" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="J24" s="64"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="58"/>
-      <c r="C25" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="62" t="s">
+      <c r="B25" s="60"/>
+      <c r="C25" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="J25" s="62"/>
-      <c r="K25" s="62"/>
-      <c r="L25" s="62"/>
-      <c r="M25" s="62"/>
-      <c r="N25" s="62"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="J25" s="64"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="64"/>
+      <c r="M25" s="64"/>
+      <c r="N25" s="64"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="58"/>
-      <c r="C26" s="61" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="62" t="s">
+      <c r="B26" s="60"/>
+      <c r="C26" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="J26" s="62"/>
-      <c r="K26" s="62"/>
-      <c r="L26" s="62"/>
-      <c r="M26" s="62"/>
-      <c r="N26" s="62"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="J26" s="64"/>
+      <c r="K26" s="64"/>
+      <c r="L26" s="64"/>
+      <c r="M26" s="64"/>
+      <c r="N26" s="64"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="58"/>
-      <c r="C27" s="61" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="62" t="s">
+      <c r="B27" s="60"/>
+      <c r="C27" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="J27" s="62"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="62"/>
-      <c r="M27" s="62"/>
-      <c r="N27" s="62"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="64" t="s">
+        <v>74</v>
+      </c>
+      <c r="J27" s="64"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="64"/>
+      <c r="N27" s="64"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="58"/>
-      <c r="C28" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="D28" s="61"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="62" t="s">
+      <c r="B28" s="60"/>
+      <c r="C28" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="J28" s="62"/>
-      <c r="K28" s="62"/>
-      <c r="L28" s="62"/>
-      <c r="M28" s="62"/>
-      <c r="N28" s="62"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="64" t="s">
+        <v>76</v>
+      </c>
+      <c r="J28" s="64"/>
+      <c r="K28" s="64"/>
+      <c r="L28" s="64"/>
+      <c r="M28" s="64"/>
+      <c r="N28" s="64"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="58"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="62" t="s">
-        <v>76</v>
-      </c>
-      <c r="J29" s="62"/>
-      <c r="K29" s="62"/>
-      <c r="L29" s="62"/>
-      <c r="M29" s="62"/>
-      <c r="N29" s="62"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="64" t="s">
+        <v>77</v>
+      </c>
+      <c r="J29" s="64"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="64"/>
+      <c r="M29" s="64"/>
+      <c r="N29" s="64"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="58"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="61"/>
-      <c r="E30" s="61"/>
-      <c r="F30" s="61"/>
-      <c r="G30" s="61"/>
-      <c r="H30" s="61"/>
-      <c r="I30" s="62" t="s">
-        <v>77</v>
-      </c>
-      <c r="J30" s="62"/>
-      <c r="K30" s="62"/>
-      <c r="L30" s="62"/>
-      <c r="M30" s="62"/>
-      <c r="N30" s="62"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="J30" s="64"/>
+      <c r="K30" s="64"/>
+      <c r="L30" s="64"/>
+      <c r="M30" s="64"/>
+      <c r="N30" s="64"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="58"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="61"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="62" t="s">
-        <v>78</v>
-      </c>
-      <c r="J31" s="62"/>
-      <c r="K31" s="62"/>
-      <c r="L31" s="62"/>
-      <c r="M31" s="62"/>
-      <c r="N31" s="62"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="63"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="J31" s="64"/>
+      <c r="K31" s="64"/>
+      <c r="L31" s="64"/>
+      <c r="M31" s="64"/>
+      <c r="N31" s="64"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="58"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="62" t="s">
-        <v>79</v>
-      </c>
-      <c r="J32" s="62"/>
-      <c r="K32" s="62"/>
-      <c r="L32" s="62"/>
-      <c r="M32" s="62"/>
-      <c r="N32" s="62"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="J32" s="64"/>
+      <c r="K32" s="64"/>
+      <c r="L32" s="64"/>
+      <c r="M32" s="64"/>
+      <c r="N32" s="64"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="58"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="61"/>
-      <c r="G33" s="61"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="J33" s="62"/>
-      <c r="K33" s="62"/>
-      <c r="L33" s="62"/>
-      <c r="M33" s="62"/>
-      <c r="N33" s="62"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="64" t="s">
+        <v>81</v>
+      </c>
+      <c r="J33" s="64"/>
+      <c r="K33" s="64"/>
+      <c r="L33" s="64"/>
+      <c r="M33" s="64"/>
+      <c r="N33" s="64"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="58"/>
-      <c r="C34" s="63"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="63"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="63"/>
-      <c r="I34" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="J34" s="64"/>
-      <c r="K34" s="64"/>
-      <c r="L34" s="64"/>
-      <c r="M34" s="64"/>
-      <c r="N34" s="64"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="66" t="s">
+        <v>82</v>
+      </c>
+      <c r="J34" s="66"/>
+      <c r="K34" s="66"/>
+      <c r="L34" s="66"/>
+      <c r="M34" s="66"/>
+      <c r="N34" s="66"/>
     </row>
     <row r="35" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="65"/>
-      <c r="C37" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="D37" s="16"/>
-      <c r="E37" s="17" t="s">
+      <c r="B37" s="67"/>
+      <c r="C37" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="F37" s="17"/>
-      <c r="G37" s="18" t="s">
+      <c r="D37" s="17"/>
+      <c r="E37" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18" t="s">
+      <c r="F37" s="18"/>
+      <c r="G37" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="J37" s="18"/>
-      <c r="K37" s="16" t="s">
+      <c r="H37" s="19"/>
+      <c r="I37" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="L37" s="16"/>
-      <c r="M37" s="16" t="s">
+      <c r="J37" s="19"/>
+      <c r="K37" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="N37" s="16"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="N37" s="17"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="65"/>
-      <c r="C38" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E38" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F38" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="H38" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J38" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="K38" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="L38" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="M38" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="N38" s="21" t="s">
-        <v>16</v>
+      <c r="B38" s="67"/>
+      <c r="C38" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="K38" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="L38" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="M38" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="N38" s="23" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="66" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" s="24" t="str">
+      <c r="B39" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,C$37,$D$11:$D$20,$B39),"")</f>
         <v/>
       </c>
-      <c r="D39" s="24" t="str">
+      <c r="D39" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,C$37,$D$11:$D$20,$B39),"")</f>
         <v/>
       </c>
-      <c r="E39" s="25" t="str">
+      <c r="E39" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,E$37,$D$11:$D$20,$B39),"")</f>
         <v/>
       </c>
-      <c r="F39" s="25" t="str">
+      <c r="F39" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,E$37,$D$11:$D$20,$B39),"")</f>
         <v/>
       </c>
-      <c r="G39" s="24" t="str">
+      <c r="G39" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,G$37,$D$11:$D$20,$B39),"")</f>
         <v/>
       </c>
-      <c r="H39" s="24" t="str">
+      <c r="H39" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,G$37,$D$11:$D$20,$B39),"")</f>
         <v/>
       </c>
-      <c r="I39" s="25" t="str">
+      <c r="I39" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,I$37,$D$11:$D$20,$B39),"")</f>
         <v/>
       </c>
-      <c r="J39" s="25" t="str">
+      <c r="J39" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,I$37,$D$11:$D$20,$B39),"")</f>
         <v/>
       </c>
-      <c r="K39" s="24" t="str">
+      <c r="K39" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,K$37,$D$11:$D$20,$B39),"")</f>
         <v/>
       </c>
-      <c r="L39" s="24" t="str">
+      <c r="L39" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,K$37,$D$11:$D$20,$B39),"")</f>
         <v/>
       </c>
-      <c r="M39" s="25" t="str">
+      <c r="M39" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,M$37,$D$11:$D$20,$B39),"")</f>
         <v/>
       </c>
-      <c r="N39" s="25" t="str">
+      <c r="N39" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,M$37,$D$11:$D$20,$B39),"")</f>
         <v/>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="66" t="s">
-        <v>89</v>
-      </c>
-      <c r="C40" s="24" t="str">
+      <c r="B40" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,C$37,$D$11:$D$20,$B40),"")</f>
         <v/>
       </c>
-      <c r="D40" s="24" t="str">
+      <c r="D40" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,C$37,$D$11:$D$20,$B40),"")</f>
         <v/>
       </c>
-      <c r="E40" s="25" t="str">
+      <c r="E40" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,E$37,$D$11:$D$20,$B40),"")</f>
         <v/>
       </c>
-      <c r="F40" s="25" t="str">
+      <c r="F40" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,E$37,$D$11:$D$20,$B40),"")</f>
         <v/>
       </c>
-      <c r="G40" s="24" t="str">
+      <c r="G40" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,G$37,$D$11:$D$20,$B40),"")</f>
         <v/>
       </c>
-      <c r="H40" s="24" t="str">
+      <c r="H40" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,G$37,$D$11:$D$20,$B40),"")</f>
         <v/>
       </c>
-      <c r="I40" s="25" t="str">
+      <c r="I40" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,I$37,$D$11:$D$20,$B40),"")</f>
         <v/>
       </c>
-      <c r="J40" s="25" t="str">
+      <c r="J40" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,I$37,$D$11:$D$20,$B40),"")</f>
         <v/>
       </c>
-      <c r="K40" s="24" t="str">
+      <c r="K40" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,K$37,$D$11:$D$20,$B40),"")</f>
         <v/>
       </c>
-      <c r="L40" s="24" t="str">
+      <c r="L40" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,K$37,$D$11:$D$20,$B40),"")</f>
         <v/>
       </c>
-      <c r="M40" s="25" t="str">
+      <c r="M40" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,M$37,$D$11:$D$20,$B40),"")</f>
         <v/>
       </c>
-      <c r="N40" s="25" t="str">
+      <c r="N40" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,M$37,$D$11:$D$20,$B40),"")</f>
         <v/>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="66" t="s">
-        <v>90</v>
-      </c>
-      <c r="C41" s="24" t="str">
+      <c r="B41" s="68" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,C$37,$D$11:$D$20,$B41),"")</f>
         <v/>
       </c>
-      <c r="D41" s="24" t="str">
+      <c r="D41" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,C$37,$D$11:$D$20,$B41),"")</f>
         <v/>
       </c>
-      <c r="E41" s="25" t="str">
+      <c r="E41" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,E$37,$D$11:$D$20,$B41),"")</f>
         <v/>
       </c>
-      <c r="F41" s="25" t="str">
+      <c r="F41" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,E$37,$D$11:$D$20,$B41),"")</f>
         <v/>
       </c>
-      <c r="G41" s="24" t="str">
+      <c r="G41" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,G$37,$D$11:$D$20,$B41),"")</f>
         <v/>
       </c>
-      <c r="H41" s="24" t="str">
+      <c r="H41" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,G$37,$D$11:$D$20,$B41),"")</f>
         <v/>
       </c>
-      <c r="I41" s="25" t="str">
+      <c r="I41" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,I$37,$D$11:$D$20,$B41),"")</f>
         <v/>
       </c>
-      <c r="J41" s="25" t="str">
+      <c r="J41" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,I$37,$D$11:$D$20,$B41),"")</f>
         <v/>
       </c>
-      <c r="K41" s="24" t="str">
+      <c r="K41" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,K$37,$D$11:$D$20,$B41),"")</f>
         <v/>
       </c>
-      <c r="L41" s="24" t="str">
+      <c r="L41" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,K$37,$D$11:$D$20,$B41),"")</f>
         <v/>
       </c>
-      <c r="M41" s="25" t="str">
+      <c r="M41" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,M$37,$D$11:$D$20,$B41),"")</f>
         <v/>
       </c>
-      <c r="N41" s="25" t="str">
+      <c r="N41" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,M$37,$D$11:$D$20,$B41),"")</f>
         <v/>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="66" t="s">
-        <v>91</v>
-      </c>
-      <c r="C42" s="24" t="str">
+      <c r="B42" s="68" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,C$37,$D$11:$D$20,$B42),"")</f>
         <v/>
       </c>
-      <c r="D42" s="24" t="str">
+      <c r="D42" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,C$37,$D$11:$D$20,$B42),"")</f>
         <v/>
       </c>
-      <c r="E42" s="25" t="str">
+      <c r="E42" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,E$37,$D$11:$D$20,$B42),"")</f>
         <v/>
       </c>
-      <c r="F42" s="25" t="str">
+      <c r="F42" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,E$37,$D$11:$D$20,$B42),"")</f>
         <v/>
       </c>
-      <c r="G42" s="24" t="str">
+      <c r="G42" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,G$37,$D$11:$D$20,$B42),"")</f>
         <v/>
       </c>
-      <c r="H42" s="24" t="str">
+      <c r="H42" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,G$37,$D$11:$D$20,$B42),"")</f>
         <v/>
       </c>
-      <c r="I42" s="25" t="str">
+      <c r="I42" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,I$37,$D$11:$D$20,$B42),"")</f>
         <v/>
       </c>
-      <c r="J42" s="25" t="str">
+      <c r="J42" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,I$37,$D$11:$D$20,$B42),"")</f>
         <v/>
       </c>
-      <c r="K42" s="24" t="str">
+      <c r="K42" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,K$37,$D$11:$D$20,$B42),"")</f>
         <v/>
       </c>
-      <c r="L42" s="24" t="str">
+      <c r="L42" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,K$37,$D$11:$D$20,$B42),"")</f>
         <v/>
       </c>
-      <c r="M42" s="25" t="str">
+      <c r="M42" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,M$37,$D$11:$D$20,$B42),"")</f>
         <v/>
       </c>
-      <c r="N42" s="25" t="str">
+      <c r="N42" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,M$37,$D$11:$D$20,$B42),"")</f>
         <v/>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="C43" s="24" t="str">
+      <c r="B43" s="68" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,C$37,$D$11:$D$20,$B43),"")</f>
         <v/>
       </c>
-      <c r="D43" s="24" t="str">
+      <c r="D43" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,C$37,$D$11:$D$20,$B43),"")</f>
         <v/>
       </c>
-      <c r="E43" s="25" t="str">
+      <c r="E43" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,E$37,$D$11:$D$20,$B43),"")</f>
         <v/>
       </c>
-      <c r="F43" s="25" t="str">
+      <c r="F43" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,E$37,$D$11:$D$20,$B43),"")</f>
         <v/>
       </c>
-      <c r="G43" s="24" t="str">
+      <c r="G43" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,G$37,$D$11:$D$20,$B43),"")</f>
         <v/>
       </c>
-      <c r="H43" s="24" t="str">
+      <c r="H43" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,G$37,$D$11:$D$20,$B43),"")</f>
         <v/>
       </c>
-      <c r="I43" s="25" t="str">
+      <c r="I43" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,I$37,$D$11:$D$20,$B43),"")</f>
         <v/>
       </c>
-      <c r="J43" s="25" t="str">
+      <c r="J43" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,I$37,$D$11:$D$20,$B43),"")</f>
         <v/>
       </c>
-      <c r="K43" s="24" t="str">
+      <c r="K43" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,K$37,$D$11:$D$20,$B43),"")</f>
         <v/>
       </c>
-      <c r="L43" s="24" t="str">
+      <c r="L43" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,K$37,$D$11:$D$20,$B43),"")</f>
         <v/>
       </c>
-      <c r="M43" s="25" t="str">
+      <c r="M43" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,M$37,$D$11:$D$20,$B43),"")</f>
         <v/>
       </c>
-      <c r="N43" s="25" t="str">
+      <c r="N43" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,M$37,$D$11:$D$20,$B43),"")</f>
         <v/>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="66" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44" s="24" t="str">
+      <c r="B44" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,C$37,$D$11:$D$20,$B44),"")</f>
         <v/>
       </c>
-      <c r="D44" s="24" t="str">
+      <c r="D44" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,C$37,$D$11:$D$20,$B44),"")</f>
         <v/>
       </c>
-      <c r="E44" s="25" t="str">
+      <c r="E44" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,E$37,$D$11:$D$20,$B44),"")</f>
         <v/>
       </c>
-      <c r="F44" s="25" t="str">
+      <c r="F44" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,E$37,$D$11:$D$20,$B44),"")</f>
         <v/>
       </c>
-      <c r="G44" s="24" t="str">
+      <c r="G44" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,G$37,$D$11:$D$20,$B44),"")</f>
         <v/>
       </c>
-      <c r="H44" s="24" t="str">
+      <c r="H44" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,G$37,$D$11:$D$20,$B44),"")</f>
         <v/>
       </c>
-      <c r="I44" s="25" t="str">
+      <c r="I44" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,I$37,$D$11:$D$20,$B44),"")</f>
         <v/>
       </c>
-      <c r="J44" s="25" t="str">
+      <c r="J44" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,I$37,$D$11:$D$20,$B44),"")</f>
         <v/>
       </c>
-      <c r="K44" s="24" t="str">
+      <c r="K44" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,K$37,$D$11:$D$20,$B44),"")</f>
         <v/>
       </c>
-      <c r="L44" s="24" t="str">
+      <c r="L44" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,K$37,$D$11:$D$20,$B44),"")</f>
         <v/>
       </c>
-      <c r="M44" s="25" t="str">
+      <c r="M44" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,M$37,$D$11:$D$20,$B44),"")</f>
         <v/>
       </c>
-      <c r="N44" s="25" t="str">
+      <c r="N44" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,M$37,$D$11:$D$20,$B44),"")</f>
         <v/>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="66" t="s">
-        <v>94</v>
-      </c>
-      <c r="C45" s="24" t="str">
+      <c r="B45" s="68" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,C$37,$D$11:$D$20,$B45),"")</f>
         <v/>
       </c>
-      <c r="D45" s="24" t="str">
+      <c r="D45" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,C$37,$D$11:$D$20,$B45),"")</f>
         <v/>
       </c>
-      <c r="E45" s="25" t="str">
+      <c r="E45" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,E$37,$D$11:$D$20,$B45),"")</f>
         <v/>
       </c>
-      <c r="F45" s="25" t="str">
+      <c r="F45" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,E$37,$D$11:$D$20,$B45),"")</f>
         <v/>
       </c>
-      <c r="G45" s="24" t="str">
+      <c r="G45" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,G$37,$D$11:$D$20,$B45),"")</f>
         <v/>
       </c>
-      <c r="H45" s="24" t="str">
+      <c r="H45" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,G$37,$D$11:$D$20,$B45),"")</f>
         <v/>
       </c>
-      <c r="I45" s="25" t="str">
+      <c r="I45" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,I$37,$D$11:$D$20,$B45),"")</f>
         <v/>
       </c>
-      <c r="J45" s="25" t="str">
+      <c r="J45" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,I$37,$D$11:$D$20,$B45),"")</f>
         <v/>
       </c>
-      <c r="K45" s="24" t="str">
+      <c r="K45" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,K$37,$D$11:$D$20,$B45),"")</f>
         <v/>
       </c>
-      <c r="L45" s="24" t="str">
+      <c r="L45" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,K$37,$D$11:$D$20,$B45),"")</f>
         <v/>
       </c>
-      <c r="M45" s="25" t="str">
+      <c r="M45" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,M$37,$D$11:$D$20,$B45),"")</f>
         <v/>
       </c>
-      <c r="N45" s="25" t="str">
+      <c r="N45" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,M$37,$D$11:$D$20,$B45),"")</f>
         <v/>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="66" t="s">
-        <v>95</v>
-      </c>
-      <c r="C46" s="24" t="str">
+      <c r="B46" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,C$37,$D$11:$D$20,$B46),"")</f>
         <v/>
       </c>
-      <c r="D46" s="24" t="str">
+      <c r="D46" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,C$37,$D$11:$D$20,$B46),"")</f>
         <v/>
       </c>
-      <c r="E46" s="25" t="str">
+      <c r="E46" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,E$37,$D$11:$D$20,$B46),"")</f>
         <v/>
       </c>
-      <c r="F46" s="25" t="str">
+      <c r="F46" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,E$37,$D$11:$D$20,$B46),"")</f>
         <v/>
       </c>
-      <c r="G46" s="24" t="str">
+      <c r="G46" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,G$37,$D$11:$D$20,$B46),"")</f>
         <v/>
       </c>
-      <c r="H46" s="24" t="str">
+      <c r="H46" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,G$37,$D$11:$D$20,$B46),"")</f>
         <v/>
       </c>
-      <c r="I46" s="25" t="str">
+      <c r="I46" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,I$37,$D$11:$D$20,$B46),"")</f>
         <v/>
       </c>
-      <c r="J46" s="25" t="str">
+      <c r="J46" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,I$37,$D$11:$D$20,$B46),"")</f>
         <v/>
       </c>
-      <c r="K46" s="24" t="str">
+      <c r="K46" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,K$37,$D$11:$D$20,$B46),"")</f>
         <v/>
       </c>
-      <c r="L46" s="24" t="str">
+      <c r="L46" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,K$37,$D$11:$D$20,$B46),"")</f>
         <v/>
       </c>
-      <c r="M46" s="25" t="str">
+      <c r="M46" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,M$37,$D$11:$D$20,$B46),"")</f>
         <v/>
       </c>
-      <c r="N46" s="25" t="str">
+      <c r="N46" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,M$37,$D$11:$D$20,$B46),"")</f>
         <v/>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="66" t="s">
-        <v>96</v>
-      </c>
-      <c r="C47" s="24" t="str">
+      <c r="B47" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,C$37,$D$11:$D$20,$B47),"")</f>
         <v/>
       </c>
-      <c r="D47" s="24" t="str">
+      <c r="D47" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,C$37,$D$11:$D$20,$B47),"")</f>
         <v/>
       </c>
-      <c r="E47" s="25" t="str">
+      <c r="E47" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,E$37,$D$11:$D$20,$B47),"")</f>
         <v/>
       </c>
-      <c r="F47" s="25" t="str">
+      <c r="F47" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,E$37,$D$11:$D$20,$B47),"")</f>
         <v/>
       </c>
-      <c r="G47" s="24" t="str">
+      <c r="G47" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,G$37,$D$11:$D$20,$B47),"")</f>
         <v/>
       </c>
-      <c r="H47" s="24" t="str">
+      <c r="H47" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,G$37,$D$11:$D$20,$B47),"")</f>
         <v/>
       </c>
-      <c r="I47" s="25" t="str">
+      <c r="I47" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,I$37,$D$11:$D$20,$B47),"")</f>
         <v/>
       </c>
-      <c r="J47" s="25" t="str">
+      <c r="J47" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,I$37,$D$11:$D$20,$B47),"")</f>
         <v/>
       </c>
-      <c r="K47" s="24" t="str">
+      <c r="K47" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,K$37,$D$11:$D$20,$B47),"")</f>
         <v/>
       </c>
-      <c r="L47" s="24" t="str">
+      <c r="L47" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,K$37,$D$11:$D$20,$B47),"")</f>
         <v/>
       </c>
-      <c r="M47" s="25" t="str">
+      <c r="M47" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,M$37,$D$11:$D$20,$B47),"")</f>
         <v/>
       </c>
-      <c r="N47" s="25" t="str">
+      <c r="N47" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,M$37,$D$11:$D$20,$B47),"")</f>
         <v/>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="66" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" s="24" t="str">
+      <c r="B48" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,C$37,$D$11:$D$20,$B48),"")</f>
         <v/>
       </c>
-      <c r="D48" s="24" t="str">
+      <c r="D48" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,C$37,$D$11:$D$20,$B48),"")</f>
         <v/>
       </c>
-      <c r="E48" s="25" t="str">
+      <c r="E48" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,E$37,$D$11:$D$20,$B48),"")</f>
         <v/>
       </c>
-      <c r="F48" s="25" t="str">
+      <c r="F48" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,E$37,$D$11:$D$20,$B48),"")</f>
         <v/>
       </c>
-      <c r="G48" s="24" t="str">
+      <c r="G48" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,G$37,$D$11:$D$20,$B48),"")</f>
         <v/>
       </c>
-      <c r="H48" s="24" t="str">
+      <c r="H48" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,G$37,$D$11:$D$20,$B48),"")</f>
         <v/>
       </c>
-      <c r="I48" s="25" t="str">
+      <c r="I48" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,I$37,$D$11:$D$20,$B48),"")</f>
         <v/>
       </c>
-      <c r="J48" s="25" t="str">
+      <c r="J48" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,I$37,$D$11:$D$20,$B48),"")</f>
         <v/>
       </c>
-      <c r="K48" s="24" t="str">
+      <c r="K48" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,K$37,$D$11:$D$20,$B48),"")</f>
         <v/>
       </c>
-      <c r="L48" s="24" t="str">
+      <c r="L48" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,K$37,$D$11:$D$20,$B48),"")</f>
         <v/>
       </c>
-      <c r="M48" s="25" t="str">
+      <c r="M48" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,M$37,$D$11:$D$20,$B48),"")</f>
         <v/>
       </c>
-      <c r="N48" s="25" t="str">
+      <c r="N48" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,M$37,$D$11:$D$20,$B48),"")</f>
         <v/>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="66" t="s">
-        <v>98</v>
-      </c>
-      <c r="C49" s="24" t="str">
+      <c r="B49" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,C$37,$D$11:$D$20,$B49),"")</f>
         <v/>
       </c>
-      <c r="D49" s="24" t="str">
+      <c r="D49" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,C$37,$D$11:$D$20,$B49),"")</f>
         <v/>
       </c>
-      <c r="E49" s="25" t="str">
+      <c r="E49" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,E$37,$D$11:$D$20,$B49),"")</f>
         <v/>
       </c>
-      <c r="F49" s="25" t="str">
+      <c r="F49" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,E$37,$D$11:$D$20,$B49),"")</f>
         <v/>
       </c>
-      <c r="G49" s="24" t="str">
+      <c r="G49" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,G$37,$D$11:$D$20,$B49),"")</f>
         <v/>
       </c>
-      <c r="H49" s="24" t="str">
+      <c r="H49" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,G$37,$D$11:$D$20,$B49),"")</f>
         <v/>
       </c>
-      <c r="I49" s="25" t="str">
+      <c r="I49" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,I$37,$D$11:$D$20,$B49),"")</f>
         <v/>
       </c>
-      <c r="J49" s="25" t="str">
+      <c r="J49" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,I$37,$D$11:$D$20,$B49),"")</f>
         <v/>
       </c>
-      <c r="K49" s="24" t="str">
+      <c r="K49" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,K$37,$D$11:$D$20,$B49),"")</f>
         <v/>
       </c>
-      <c r="L49" s="24" t="str">
+      <c r="L49" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,K$37,$D$11:$D$20,$B49),"")</f>
         <v/>
       </c>
-      <c r="M49" s="25" t="str">
+      <c r="M49" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,M$37,$D$11:$D$20,$B49),"")</f>
         <v/>
       </c>
-      <c r="N49" s="25" t="str">
+      <c r="N49" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,M$37,$D$11:$D$20,$B49),"")</f>
         <v/>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="66" t="s">
-        <v>99</v>
-      </c>
-      <c r="C50" s="24" t="str">
+      <c r="B50" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="C50" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,C$37,$D$11:$D$20,$B50),"")</f>
         <v/>
       </c>
-      <c r="D50" s="24" t="str">
+      <c r="D50" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,C$37,$D$11:$D$20,$B50),"")</f>
         <v/>
       </c>
-      <c r="E50" s="25" t="str">
+      <c r="E50" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,E$37,$D$11:$D$20,$B50),"")</f>
         <v/>
       </c>
-      <c r="F50" s="25" t="str">
+      <c r="F50" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,E$37,$D$11:$D$20,$B50),"")</f>
         <v/>
       </c>
-      <c r="G50" s="24" t="str">
+      <c r="G50" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,G$37,$D$11:$D$20,$B50),"")</f>
         <v/>
       </c>
-      <c r="H50" s="24" t="str">
+      <c r="H50" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,G$37,$D$11:$D$20,$B50),"")</f>
         <v/>
       </c>
-      <c r="I50" s="25" t="str">
+      <c r="I50" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,I$37,$D$11:$D$20,$B50),"")</f>
         <v/>
       </c>
-      <c r="J50" s="25" t="str">
+      <c r="J50" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,I$37,$D$11:$D$20,$B50),"")</f>
         <v/>
       </c>
-      <c r="K50" s="24" t="str">
+      <c r="K50" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,K$37,$D$11:$D$20,$B50),"")</f>
         <v/>
       </c>
-      <c r="L50" s="24" t="str">
+      <c r="L50" s="26" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,K$37,$D$11:$D$20,$B50),"")</f>
         <v/>
       </c>
-      <c r="M50" s="25" t="str">
+      <c r="M50" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($E$11:$E$20,$C$11:$C$20,M$37,$D$11:$D$20,$B50),"")</f>
         <v/>
       </c>
-      <c r="N50" s="25" t="str">
+      <c r="N50" s="27" t="str">
         <f aca="false">IFERROR(AVERAGEIFS($F$11:$F$20,$C$11:$C$20,M$37,$D$11:$D$20,$B50),"")</f>
         <v/>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="67"/>
-      <c r="C51" s="68" t="s">
-        <v>100</v>
-      </c>
-      <c r="D51" s="68"/>
-      <c r="E51" s="68"/>
-      <c r="F51" s="68"/>
-      <c r="G51" s="68"/>
-      <c r="H51" s="68"/>
-      <c r="I51" s="68"/>
-      <c r="J51" s="68"/>
-      <c r="K51" s="68"/>
-      <c r="L51" s="68"/>
-      <c r="M51" s="68"/>
-      <c r="N51" s="68"/>
-    </row>
+      <c r="B51" s="69"/>
+      <c r="C51" s="70" t="s">
+        <v>101</v>
+      </c>
+      <c r="D51" s="70"/>
+      <c r="E51" s="70"/>
+      <c r="F51" s="70"/>
+      <c r="G51" s="70"/>
+      <c r="H51" s="70"/>
+      <c r="I51" s="70"/>
+      <c r="J51" s="70"/>
+      <c r="K51" s="70"/>
+      <c r="L51" s="70"/>
+      <c r="M51" s="70"/>
+      <c r="N51" s="70"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="58">
     <mergeCell ref="B2:N2"/>
@@ -4643,7 +4663,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="T9:Z14 C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4656,194 +4676,194 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="69" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
+      <c r="A1" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="70" t="s">
-        <v>101</v>
+      <c r="B2" s="72" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="71" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
+      <c r="A3" s="73" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
     </row>
     <row r="4" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="72"/>
-      <c r="B4" s="73" t="s">
+      <c r="A4" s="74"/>
+      <c r="B4" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="74" t="s">
-        <v>103</v>
+      <c r="C4" s="76" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="72"/>
-      <c r="B5" s="73" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" s="74" t="s">
+      <c r="A5" s="74"/>
+      <c r="B5" s="75" t="s">
         <v>105</v>
       </c>
+      <c r="C5" s="76" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="72"/>
-      <c r="B6" s="73" t="s">
+      <c r="A6" s="74"/>
+      <c r="B6" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="74" t="s">
-        <v>106</v>
+      <c r="C6" s="76" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="72"/>
-      <c r="B7" s="73" t="s">
-        <v>107</v>
-      </c>
-      <c r="C7" s="74" t="s">
+      <c r="A7" s="74"/>
+      <c r="B7" s="75" t="s">
         <v>108</v>
       </c>
+      <c r="C7" s="76" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="49.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="72"/>
-      <c r="B8" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" s="74" t="s">
+      <c r="A8" s="74"/>
+      <c r="B8" s="75" t="s">
         <v>110</v>
       </c>
+      <c r="C8" s="76" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="72"/>
-      <c r="B9" s="73" t="s">
-        <v>111</v>
-      </c>
-      <c r="C9" s="74" t="s">
+      <c r="A9" s="74"/>
+      <c r="B9" s="75" t="s">
         <v>112</v>
       </c>
+      <c r="C9" s="76" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="75"/>
+      <c r="B10" s="77"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="76" t="s">
-        <v>113</v>
-      </c>
-      <c r="B11" s="77"/>
-      <c r="C11" s="78"/>
+      <c r="A11" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
     </row>
     <row r="12" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="78"/>
-      <c r="B12" s="73" t="s">
-        <v>114</v>
-      </c>
-      <c r="C12" s="74" t="s">
+      <c r="A12" s="80"/>
+      <c r="B12" s="75" t="s">
         <v>115</v>
       </c>
+      <c r="C12" s="76" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="78"/>
-      <c r="B13" s="73" t="s">
-        <v>116</v>
-      </c>
-      <c r="C13" s="74" t="s">
+      <c r="A13" s="80"/>
+      <c r="B13" s="75" t="s">
         <v>117</v>
       </c>
+      <c r="C13" s="76" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="78"/>
-      <c r="B14" s="73" t="s">
-        <v>118</v>
-      </c>
-      <c r="C14" s="74" t="s">
+      <c r="A14" s="80"/>
+      <c r="B14" s="75" t="s">
         <v>119</v>
       </c>
+      <c r="C14" s="76" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="78"/>
-      <c r="B15" s="73" t="s">
-        <v>120</v>
-      </c>
-      <c r="C15" s="74" t="s">
+      <c r="A15" s="80"/>
+      <c r="B15" s="75" t="s">
         <v>121</v>
       </c>
+      <c r="C15" s="76" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="78"/>
-      <c r="B16" s="73" t="s">
-        <v>122</v>
-      </c>
-      <c r="C16" s="74" t="s">
+      <c r="A16" s="80"/>
+      <c r="B16" s="75" t="s">
         <v>123</v>
       </c>
+      <c r="C16" s="76" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="78"/>
-      <c r="B17" s="73" t="s">
-        <v>124</v>
-      </c>
-      <c r="C17" s="74" t="s">
+      <c r="A17" s="80"/>
+      <c r="B17" s="75" t="s">
         <v>125</v>
       </c>
+      <c r="C17" s="76" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="78"/>
-      <c r="B18" s="73" t="s">
-        <v>126</v>
-      </c>
-      <c r="C18" s="74" t="s">
+      <c r="A18" s="80"/>
+      <c r="B18" s="75" t="s">
         <v>127</v>
       </c>
+      <c r="C18" s="76" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="78"/>
-      <c r="B19" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="C19" s="74" t="s">
+      <c r="A19" s="80"/>
+      <c r="B19" s="75" t="s">
         <v>129</v>
       </c>
+      <c r="C19" s="76" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="78"/>
-      <c r="B20" s="73" t="s">
-        <v>130</v>
-      </c>
-      <c r="C20" s="74" t="s">
+      <c r="A20" s="80"/>
+      <c r="B20" s="75" t="s">
         <v>131</v>
       </c>
+      <c r="C20" s="76" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="78"/>
-      <c r="B21" s="73" t="s">
-        <v>132</v>
-      </c>
-      <c r="C21" s="74" t="s">
+      <c r="A21" s="80"/>
+      <c r="B21" s="75" t="s">
         <v>133</v>
       </c>
+      <c r="C21" s="76" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="78"/>
-      <c r="B22" s="73" t="s">
-        <v>134</v>
-      </c>
-      <c r="C22" s="74" t="s">
+      <c r="A22" s="80"/>
+      <c r="B22" s="75" t="s">
         <v>135</v>
       </c>
+      <c r="C22" s="76" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="78"/>
-      <c r="B23" s="73" t="s">
-        <v>136</v>
-      </c>
-      <c r="C23" s="74" t="s">
+      <c r="A23" s="80"/>
+      <c r="B23" s="75" t="s">
         <v>137</v>
+      </c>
+      <c r="C23" s="76" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>